<commit_message>
make_checklist generates markdown files based on the output from CTPL
</commit_message>
<xml_diff>
--- a/vignettes/results.xlsx
+++ b/vignettes/results.xlsx
@@ -12,9 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
-  <si>
-    <t xml:space="preserve">TAXA_NAME</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+  <si>
+    <t xml:space="preserve">YOUR_SEARCH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPECIES_CN</t>
   </si>
   <si>
     <t xml:space="preserve">SPECIES</t>
@@ -177,6 +180,9 @@
   </si>
   <si>
     <t xml:space="preserve">300-2100(-2100)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">绿樟</t>
   </si>
   <si>
     <t xml:space="preserve">网脉实蕨</t>
@@ -587,10 +593,13 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
@@ -626,18 +635,21 @@
         <v>26</v>
       </c>
       <c r="M2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N2" t="s">
         <v>27</v>
       </c>
       <c r="O2" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="P2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
         <v>29</v>
@@ -667,10 +679,10 @@
         <v>37</v>
       </c>
       <c r="K3" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="L3" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="M3" t="s">
         <v>39</v>
@@ -680,11 +692,14 @@
       </c>
       <c r="O3" t="s">
         <v>41</v>
+      </c>
+      <c r="P3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
         <v>43</v>
@@ -714,66 +729,92 @@
         <v>51</v>
       </c>
       <c r="K4" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="L4" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="M4" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="N4" t="s">
         <v>53</v>
       </c>
       <c r="O4" t="s">
         <v>54</v>
+      </c>
+      <c r="P4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" t="s">
         <v>56</v>
       </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
         <v>57</v>
       </c>
-      <c r="E5" t="s">
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" t="s">
         <v>58</v>
       </c>
-      <c r="F5" t="s">
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
         <v>59</v>
       </c>
-      <c r="G5" t="s">
+      <c r="F6" t="s">
         <v>60</v>
       </c>
-      <c r="H5" t="s">
+      <c r="G6" t="s">
         <v>61</v>
       </c>
-      <c r="I5" t="s">
+      <c r="H6" t="s">
         <v>62</v>
       </c>
-      <c r="J5" t="s">
+      <c r="I6" t="s">
         <v>63</v>
       </c>
-      <c r="K5" t="s">
+      <c r="J6" t="s">
         <v>64</v>
       </c>
-      <c r="L5" t="s">
+      <c r="K6" t="s">
         <v>65</v>
       </c>
-      <c r="M5" t="s">
-        <v>39</v>
-      </c>
-      <c r="N5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O5" t="s">
-        <v>26</v>
+      <c r="L6" t="s">
+        <v>66</v>
+      </c>
+      <c r="M6" t="s">
+        <v>67</v>
+      </c>
+      <c r="N6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O6" t="s">
+        <v>27</v>
+      </c>
+      <c r="P6" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>